<commit_message>
Modified project two documents. Added project four documents.
</commit_message>
<xml_diff>
--- a/project2/servo calibration-workdelta.xlsx
+++ b/project2/servo calibration-workdelta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="10785" windowHeight="6765"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="10785" windowHeight="6765" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t xml:space="preserve"> Measured T Pass</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Ki</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -29164,7 +29167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -29274,8 +29277,8 @@
       <c r="C10" s="14">
         <v>3.1812500000000004</v>
       </c>
-      <c r="D10" s="5">
-        <v>4.1390000000000002</v>
+      <c r="D10" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="29">
@@ -29298,9 +29301,9 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D14">
+      <c r="D14" t="e">
         <f>1/D10</f>
-        <v>0.24160425223483931</v>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -47922,7 +47925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>

</xml_diff>